<commit_message>
Pred testy na A7
</commit_message>
<xml_diff>
--- a/TADtasks/ELSW_3448/ELSW-3448_TAD_MPPC_ETD.xlsx
+++ b/TADtasks/ELSW_3448/ELSW-3448_TAD_MPPC_ETD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3602951-3513-41FC-BC78-B37E9AD4B3FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F3A45F-443B-47C8-A322-4A6B0EABAA63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4272" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="4272" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MPPC ETD" sheetId="2" r:id="rId1"/>
@@ -1756,10 +1756,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1771,13 +1778,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2171,8 +2171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2BAFA7D-B17F-4BAB-8749-750D6EBA6C6C}">
   <dimension ref="A4:P234"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="D144" sqref="D144"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="G140" sqref="G140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2663,11 +2663,11 @@
       </c>
     </row>
     <row r="130" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C130" s="29" t="s">
+      <c r="C130" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D130" s="29"/>
-      <c r="E130" s="29"/>
+      <c r="D130" s="33"/>
+      <c r="E130" s="33"/>
       <c r="G130">
         <v>2.6</v>
       </c>
@@ -2676,11 +2676,11 @@
       </c>
     </row>
     <row r="131" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C131" s="30" t="s">
+      <c r="C131" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D131" s="30"/>
-      <c r="E131" s="30"/>
+      <c r="D131" s="34"/>
+      <c r="E131" s="34"/>
       <c r="G131">
         <v>110</v>
       </c>
@@ -3046,7 +3046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E8F5F2-E89E-4F27-9DDA-C2ECCDDF7403}">
   <dimension ref="A2:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -3070,27 +3070,27 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="29" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="29" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="29" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="29" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="29" t="s">
         <v>253</v>
       </c>
     </row>
@@ -3098,15 +3098,15 @@
       <c r="B10" t="s">
         <v>261</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="31" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="29" t="s">
         <v>255</v>
       </c>
       <c r="C11">
@@ -3114,7 +3114,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="29" t="s">
         <v>256</v>
       </c>
       <c r="C13">
@@ -3122,7 +3122,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="29" t="s">
         <v>257</v>
       </c>
       <c r="C14">
@@ -3130,7 +3130,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="29" t="s">
         <v>260</v>
       </c>
     </row>
@@ -3140,7 +3140,7 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="29" t="s">
         <v>256</v>
       </c>
       <c r="C18">
@@ -3148,7 +3148,7 @@
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="29" t="s">
         <v>257</v>
       </c>
       <c r="C19">
@@ -3156,7 +3156,7 @@
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="29" t="s">
         <v>260</v>
       </c>
     </row>
@@ -3170,7 +3170,7 @@
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="29" t="s">
         <v>256</v>
       </c>
       <c r="C23">
@@ -3178,7 +3178,7 @@
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="29" t="s">
         <v>257</v>
       </c>
       <c r="C24">
@@ -3186,7 +3186,7 @@
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="29" t="s">
         <v>260</v>
       </c>
     </row>
@@ -3200,7 +3200,7 @@
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="29" t="s">
         <v>256</v>
       </c>
       <c r="C28">
@@ -3208,7 +3208,7 @@
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="29" t="s">
         <v>257</v>
       </c>
       <c r="C29">
@@ -3216,7 +3216,7 @@
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="29" t="s">
         <v>260</v>
       </c>
     </row>
@@ -3233,7 +3233,7 @@
       <c r="A37" t="s">
         <v>183</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="30" t="s">
         <v>259</v>
       </c>
       <c r="D37" s="26" t="s">
@@ -3241,17 +3241,17 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="29" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="29" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="29" t="s">
         <v>266</v>
       </c>
       <c r="D40">
@@ -3260,7 +3260,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="29" t="s">
         <v>255</v>
       </c>
       <c r="D41">
@@ -3268,7 +3268,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="29" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3388,11 +3388,11 @@
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
       <c r="D32" s="13"/>
       <c r="E32" s="12" t="s">
         <v>28</v>
@@ -3404,10 +3404,10 @@
         <v>30</v>
       </c>
       <c r="H32" s="13"/>
-      <c r="I32" s="34" t="s">
+      <c r="I32" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="J32" s="34"/>
+      <c r="J32" s="35"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
@@ -3436,10 +3436,10 @@
       <c r="Q33" s="13"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="31"/>
+      <c r="B34" s="36"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
       <c r="E34" s="14">
@@ -3452,24 +3452,24 @@
         <v>-1.2679</v>
       </c>
       <c r="H34" s="13"/>
-      <c r="I34" s="32" t="s">
+      <c r="I34" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32"/>
-      <c r="P34" s="32"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="37"/>
+      <c r="O34" s="37"/>
+      <c r="P34" s="37"/>
       <c r="Q34" s="13"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
       <c r="D35" s="13"/>
       <c r="E35" s="14">
         <v>25</v>
@@ -3481,24 +3481,24 @@
         <v>24.018000000000001</v>
       </c>
       <c r="H35" s="13"/>
-      <c r="I35" s="32" t="s">
+      <c r="I35" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="32"/>
-      <c r="P35" s="32"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="37"/>
+      <c r="P35" s="37"/>
       <c r="Q35" s="13"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
       <c r="D36" s="13"/>
       <c r="E36" s="14">
         <v>50</v>
@@ -3510,24 +3510,24 @@
         <v>48.768000000000001</v>
       </c>
       <c r="H36" s="13"/>
-      <c r="I36" s="32" t="s">
+      <c r="I36" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="37"/>
+      <c r="N36" s="37"/>
+      <c r="O36" s="37"/>
+      <c r="P36" s="37"/>
       <c r="Q36" s="13"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
       <c r="D37" s="13"/>
       <c r="E37" s="14">
         <v>30</v>
@@ -3539,24 +3539,24 @@
         <v>30.702000000000002</v>
       </c>
       <c r="H37" s="13"/>
-      <c r="I37" s="32" t="s">
+      <c r="I37" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="32"/>
-      <c r="P37" s="32"/>
-      <c r="Q37" s="32"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37"/>
+      <c r="Q37" s="37"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
       <c r="D38" s="13"/>
       <c r="E38" s="14">
         <v>110</v>
@@ -3564,28 +3564,28 @@
       <c r="F38" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G38" s="33" t="s">
+      <c r="G38" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="H38" s="33"/>
-      <c r="I38" s="32" t="s">
+      <c r="H38" s="38"/>
+      <c r="I38" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
-      <c r="Q38" s="32"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="37"/>
+      <c r="O38" s="37"/>
+      <c r="P38" s="37"/>
+      <c r="Q38" s="37"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
       <c r="D39" s="13"/>
       <c r="E39" s="14">
         <v>2.6</v>
@@ -3598,23 +3598,23 @@
         <v>0</v>
       </c>
       <c r="H39" s="13"/>
-      <c r="I39" s="32" t="s">
+      <c r="I39" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
-      <c r="P39" s="32"/>
-      <c r="Q39" s="32"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="P39" s="37"/>
+      <c r="Q39" s="37"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B40" s="31"/>
+      <c r="B40" s="36"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
       <c r="E40" s="14">
@@ -3627,11 +3627,11 @@
         <v>47</v>
       </c>
       <c r="H40" s="13"/>
-      <c r="I40" s="32" t="s">
+      <c r="I40" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="37"/>
       <c r="L40" s="13"/>
       <c r="M40" s="13"/>
       <c r="N40" s="13"/>
@@ -4045,12 +4045,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="I34:P34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="I35:P35"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="I39:Q39"/>
     <mergeCell ref="A40:B40"/>
@@ -4062,6 +4056,12 @@
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="I38:Q38"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="I34:P34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="I35:P35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A62" r:id="rId1" display="mailto:pavel.stejskal@fei.com" xr:uid="{9047D5E3-CAD2-4293-BDD0-9580F005C129}"/>

</xml_diff>